<commit_message>
Last commit. Good luck bro, stay strong(11:53 18-12-2023)^^
</commit_message>
<xml_diff>
--- a/server_nodejs/question_import_result.xlsx
+++ b/server_nodejs/question_import_result.xlsx
@@ -404,7 +404,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Kết quả import người dùng vào lớp tín chỉ</v>
+        <v>Kết quả import câu hỏi</v>
       </c>
       <c r="B1" t="str">
         <v/>
@@ -415,15 +415,15 @@
         <v>Thời gian</v>
       </c>
       <c r="B2" t="str">
-        <v>Sat Dec 16 2023 19:25:21 GMT+0700 (Indochina Time)</v>
+        <v>Mon Dec 18 2023 16:59:31 GMT+0700 (Indochina Time)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Tổng số tài khoản được import</v>
+        <v>Tổng câu hỏi</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -431,7 +431,7 @@
         <v>Thành công</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -439,7 +439,7 @@
         <v>Thất bại</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>